<commit_message>
Add age for Brooke
</commit_message>
<xml_diff>
--- a/data/2020-02-17/Senior Cubers Worldwide - Weekly Competition - 2020-02-17.xlsx
+++ b/data/2020-02-17/Senior Cubers Worldwide - Weekly Competition - 2020-02-17.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-weekly-comp\data\2020-02-17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-02-17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD5AE7B-3D41-4F44-AF9B-B774F98B56A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4E9DA3-2FBA-447A-A3A3-F7F8C12AFCFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -853,7 +853,7 @@
   <dimension ref="A1:K1032"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1833,7 +1833,7 @@
         <v>95</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="D30" s="15">
         <v>58.52</v>

</xml_diff>